<commit_message>
Structural arrangement & formating
</commit_message>
<xml_diff>
--- a/input/rectal_dataset_full.xlsx
+++ b/input/rectal_dataset_full.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/90b7a5025e4172ad/rectal_chemo_vs_surveillance/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="8_{5CF9A380-9EAA-5F40-8663-BD93FEF6C00E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2D857B9E-CDD9-DF40-AE16-95D54EE3B703}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="8_{5CF9A380-9EAA-5F40-8663-BD93FEF6C00E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A81F57E4-9A68-3746-A793-B224B77A03F5}"/>
   <bookViews>
-    <workbookView xWindow="9340" yWindow="3700" windowWidth="34080" windowHeight="21440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9340" yWindow="3700" windowWidth="41860" windowHeight="23080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -10554,7 +10554,7 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="368">
+  <cellXfs count="369">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -11609,6 +11609,9 @@
     <xf numFmtId="0" fontId="13" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -11935,10 +11938,10 @@
   <dimension ref="A1:CA1541"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="AR55" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="AW72" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BB57" sqref="BB57"/>
+      <selection pane="bottomRight" activeCell="BB73" sqref="BB73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23665,7 +23668,7 @@
         <v>174</v>
       </c>
       <c r="BB73" s="226">
-        <v>42547</v>
+        <v>44008</v>
       </c>
       <c r="BC73" s="246"/>
       <c r="BD73" s="246"/>
@@ -35995,7 +35998,7 @@
       <c r="BC146" s="170"/>
     </row>
     <row r="147" spans="1:55" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A147" s="238" t="s">
+      <c r="A147" s="368" t="s">
         <v>1472</v>
       </c>
       <c r="B147" s="260">
@@ -37187,7 +37190,7 @@
       <c r="BC154" s="170"/>
     </row>
     <row r="155" spans="1:55" ht="176" x14ac:dyDescent="0.2">
-      <c r="A155" s="238" t="s">
+      <c r="A155" s="368" t="s">
         <v>1548</v>
       </c>
       <c r="B155" s="260">

</xml_diff>